<commit_message>
adding results, removing compressed files
</commit_message>
<xml_diff>
--- a/Compression results.xlsx
+++ b/Compression results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdel/PycharmProjects/cor-space-config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73BAAD2B-FE22-6F40-B38D-738BCD08337B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B4F5D9-13C6-1C45-A340-9BBA5FA5C98F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44200" yWindow="7820" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{EA6EA9B5-B5A8-E14B-A1A8-570F267023DC}"/>
+    <workbookView xWindow="44200" yWindow="7720" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{EA6EA9B5-B5A8-E14B-A1A8-570F267023DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Baselines " sheetId="5" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="algo vs. algo" sheetId="6" r:id="rId3"/>
     <sheet name="sparsity level" sheetId="10" r:id="rId4"/>
     <sheet name="correaltion threshold" sheetId="11" r:id="rId5"/>
-    <sheet name="tricklet size" sheetId="12" r:id="rId6"/>
+    <sheet name="tricklet length" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>Regression (Eichinger et. al 2015)</t>
   </si>
@@ -191,12 +191,6 @@
     <t xml:space="preserve">Tricklet length </t>
   </si>
   <si>
-    <t>Ts Length</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nb Ts </t>
-  </si>
-  <si>
     <t>CinCECGTorso (test)</t>
   </si>
   <si>
@@ -210,9 +204,6 @@
   </si>
   <si>
     <t>Matching pursuit algorithm</t>
-  </si>
-  <si>
-    <t>Comperssion time</t>
   </si>
   <si>
     <t>Reconstruction time</t>
@@ -286,32 +277,41 @@
     <t>* initial size/ new size</t>
   </si>
   <si>
-    <t xml:space="preserve"> (tristan vs. ours)</t>
-  </si>
-  <si>
     <t>MSE Tristan</t>
   </si>
   <si>
     <t>MSE ours</t>
   </si>
   <si>
-    <t>Compression ratio Tristan</t>
-  </si>
-  <si>
-    <t>Compression ratio ours</t>
-  </si>
-  <si>
     <t>Comp%Reconst time Tristan</t>
   </si>
   <si>
     <t>Comp%Reconst time ours</t>
+  </si>
+  <si>
+    <t>Compression ratio Tristan*</t>
+  </si>
+  <si>
+    <t>Compression ratio ours*</t>
+  </si>
+  <si>
+    <t>PigAirwayPressure_TRAIN</t>
+  </si>
+  <si>
+    <t>207, 2001</t>
+  </si>
+  <si>
+    <t>ACSF1_TRAIN</t>
+  </si>
+  <si>
+    <t>(99, 1461)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -346,6 +346,13 @@
     <font>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -426,11 +433,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,14 +489,35 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -811,7 +836,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F1F3C3F-3BD3-A14E-B668-D1F985F2737F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -822,53 +847,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>64</v>
+      <c r="A1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="24" t="s">
-        <v>65</v>
+      <c r="A2" s="23" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="23"/>
+      <c r="B3" s="22"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="22"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="23"/>
+      <c r="B5" s="22"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="22"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>6</v>
       </c>
     </row>
@@ -885,381 +910,381 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="64.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="38" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="64.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>53</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>811</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <f t="shared" ref="E2:E7" si="0">B2*C2</f>
         <v>42983</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>3000</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>426</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <f t="shared" si="0"/>
         <v>1278000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="8">
+    <row r="4" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7">
         <v>1380</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>1639</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="9">
         <f t="shared" si="0"/>
         <v>2261820</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>208</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>2000</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="10">
+      <c r="D5" s="10"/>
+      <c r="E5" s="9">
         <f t="shared" si="0"/>
         <v>416000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>29</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>19735</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <f t="shared" si="0"/>
         <v>572315</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>15</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>295719</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="9">
         <f t="shared" si="0"/>
         <v>4435785</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>3582</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>945</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <f t="shared" ref="E8:E12" si="1">B8*C8</f>
         <v>3384990</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>6164</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>152</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f t="shared" si="1"/>
         <v>936928</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>4000</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>128</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <f t="shared" si="1"/>
         <v>512000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>8236</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>1024</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <f t="shared" si="1"/>
         <v>8433664</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>100</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>1460</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <f t="shared" si="1"/>
         <v>146000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:5" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>119</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="14">
         <v>3000</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="15">
         <f t="shared" ref="E13:E21" si="2">B13*C13</f>
         <v>357000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>600</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>1500</v>
       </c>
-      <c r="E14" s="7">
+      <c r="E14" s="6">
         <f t="shared" si="2"/>
         <v>900000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>52</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>3850505</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E15" s="6">
         <f t="shared" si="2"/>
         <v>200226260</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>12</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>63000000</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="7">
+      <c r="E16" s="6">
         <f t="shared" si="2"/>
         <v>756000000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>86</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>52854</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <f t="shared" si="2"/>
         <v>4545444</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:5" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="12">
+      <c r="B18" s="11">
         <v>13</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>43824</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <f t="shared" si="2"/>
         <v>569712</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>77</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>140000</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <f t="shared" si="2"/>
         <v>10780000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>13</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>230318</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <f t="shared" si="2"/>
         <v>2994134</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>20</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>4095000</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <f t="shared" si="2"/>
         <v>81900000</v>
       </c>
@@ -1279,6 +1304,7 @@
     <hyperlink ref="D7" r:id="rId11" xr:uid="{F586B74C-69C3-234C-A172-1C832FB93153}"/>
     <hyperlink ref="D10" r:id="rId12" xr:uid="{62C32C0C-4948-094F-8DC8-89B612203487}"/>
     <hyperlink ref="D9" r:id="rId13" xr:uid="{C792C2CF-CA01-1944-ACE2-ED5FB859DBB8}"/>
+    <hyperlink ref="D4" r:id="rId14" xr:uid="{F6C3274B-8834-F944-B79C-20474B09A6BF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1289,119 +1315,119 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F94416DE-30B7-E345-8186-BD11BDED46A2}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="19" customWidth="1"/>
-    <col min="3" max="4" width="12.5" style="19" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="17.5" style="18" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="18" customWidth="1"/>
+    <col min="3" max="4" width="12.5" style="18" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" style="18" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="18" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="21"/>
+      <c r="B1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="20"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="20"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="21" t="s">
+      <c r="C4" s="20"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="C5" s="20"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="20"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="C7" s="20"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="20">
+        <v>100</v>
+      </c>
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B14" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="B15" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A4" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="21">
-        <v>0.95</v>
-      </c>
-      <c r="C5" s="21"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="21"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="21"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="21">
-        <v>100</v>
-      </c>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B14" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="19" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="B16" s="19" t="s">
-        <v>65</v>
+      <c r="B16" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1413,267 +1439,410 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F24F4C8-E6FE-784E-B1A1-5B7567BD0581}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" style="19" customWidth="1"/>
-    <col min="2" max="4" width="17" style="19" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="19"/>
-    <col min="6" max="6" width="20.6640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="18.83203125" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="19"/>
+    <col min="1" max="1" width="17.1640625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" style="18" customWidth="1"/>
+    <col min="4" max="4" width="17" style="18" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="18"/>
+    <col min="6" max="6" width="20.6640625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
+      <c r="B1" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
+      <c r="B2" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="20">
+        <v>14</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A4" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="21">
-        <v>14</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A5" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="21">
-        <v>0.95</v>
-      </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A6" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A7" s="21" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B8" s="20">
+        <v>100</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A9" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A8" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B8" s="21">
-        <v>100</v>
-      </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A9" s="19" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="E12" s="17" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A12" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>82</v>
+      <c r="F12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A13" s="19">
+      <c r="A13" s="18">
         <v>1</v>
       </c>
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>7.9</v>
       </c>
-      <c r="C13" s="19">
+      <c r="C13" s="18">
         <v>6.61</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>1.8269</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <v>2.0186999999999999</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="18">
         <v>9.7799999999999994</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="18">
         <v>41.76</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A14" s="19">
+      <c r="A14" s="18">
         <v>2</v>
       </c>
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="18">
         <v>5.95</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="18">
         <v>0.68108999999999997</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="18">
         <v>0.80971000000000004</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="18">
         <v>15.5</v>
       </c>
-      <c r="G14" s="19">
+      <c r="G14" s="18">
         <v>43.72</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A15" s="19">
+      <c r="A15" s="18">
         <v>3</v>
       </c>
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>2.7</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="18">
         <v>5.67</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>0.25777</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="18">
         <v>0.34228999999999998</v>
       </c>
-      <c r="F15" s="19">
+      <c r="F15" s="18">
         <v>22.18</v>
       </c>
-      <c r="G15" s="19">
+      <c r="G15" s="18">
         <v>51.27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A16" s="19">
+      <c r="A16" s="18">
         <v>4</v>
       </c>
-      <c r="B16" s="19">
+      <c r="B16" s="18">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="C16" s="18">
+        <v>5.17</v>
+      </c>
+      <c r="D16" s="18">
+        <v>9.9419999999999994E-2</v>
+      </c>
+      <c r="E16" s="18">
+        <v>0.15548000000000001</v>
+      </c>
+      <c r="F16" s="18">
+        <v>27.83</v>
+      </c>
+      <c r="G16" s="18">
+        <v>56.62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A17" s="18">
+        <v>5</v>
+      </c>
+      <c r="B17" s="18">
         <v>1.63</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C17" s="18">
         <v>4.76</v>
       </c>
-      <c r="D16" s="19">
-        <v>4.8591000000000002E-2</v>
-      </c>
-      <c r="E16" s="19">
-        <v>9.0674000000000005E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="19">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="19">
+      <c r="D17" s="18">
+        <v>5.0294999999999999E-2</v>
+      </c>
+      <c r="E17" s="18">
+        <v>9.2800999999999995E-2</v>
+      </c>
+      <c r="F17" s="18">
+        <v>32.68</v>
+      </c>
+      <c r="G17" s="18">
+        <v>60.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A18" s="18">
         <v>6</v>
       </c>
-      <c r="B18" s="19">
+      <c r="B18" s="18">
         <v>1.35</v>
       </c>
-      <c r="C18" s="19">
-        <v>4.4000000000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="19">
+      <c r="C18" s="18">
+        <v>4.41</v>
+      </c>
+      <c r="D18" s="18">
+        <v>2.0784E-2</v>
+      </c>
+      <c r="E18" s="18">
+        <v>5.1355999999999999E-2</v>
+      </c>
+      <c r="F18" s="18">
+        <v>38.200000000000003</v>
+      </c>
+      <c r="G18" s="18">
+        <v>65.73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A19" s="18">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="19">
+      <c r="B19" s="18">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C19" s="18">
+        <v>4.25</v>
+      </c>
+      <c r="D19" s="18">
+        <v>6.1311999999999998E-3</v>
+      </c>
+      <c r="E19" s="18">
+        <v>2.7574000000000001E-2</v>
+      </c>
+      <c r="F19" s="18">
+        <v>46.86</v>
+      </c>
+      <c r="G19" s="18">
+        <v>73.39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A20" s="18">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="19">
+      <c r="B20" s="18">
+        <v>1.01</v>
+      </c>
+      <c r="C20" s="18">
+        <v>3.97</v>
+      </c>
+      <c r="D20" s="18">
+        <v>2.0072E-2</v>
+      </c>
+      <c r="E20" s="18">
+        <v>2.5839999999999999E-3</v>
+      </c>
+      <c r="F20" s="18">
+        <v>51.94</v>
+      </c>
+      <c r="G20" s="18">
+        <v>76.86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A21" s="18">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="19">
+      <c r="B21" s="18">
+        <v>0.79</v>
+      </c>
+      <c r="C21" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="D21" s="18">
+        <v>1.1377E-4</v>
+      </c>
+      <c r="E21" s="18">
+        <v>1.2269E-2</v>
+      </c>
+      <c r="F21" s="18">
+        <v>63.55</v>
+      </c>
+      <c r="G21" s="18">
+        <v>87.43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A22" s="18">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="19">
+      <c r="B22" s="18">
+        <v>0.67</v>
+      </c>
+      <c r="C22" s="18">
+        <v>3.21</v>
+      </c>
+      <c r="D22" s="26">
+        <v>2.9842000000000002E-6</v>
+      </c>
+      <c r="E22" s="18">
+        <v>1.1161000000000001E-2</v>
+      </c>
+      <c r="F22" s="18">
+        <v>73.540000000000006</v>
+      </c>
+      <c r="G22" s="18">
+        <v>96.97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A23" s="18">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="19">
+      <c r="B23" s="18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C23" s="18">
+        <v>2.98</v>
+      </c>
+      <c r="D23" s="26">
+        <v>2.0546999999999999E-37</v>
+      </c>
+      <c r="E23" s="18">
+        <v>1.1062000000000001E-2</v>
+      </c>
+      <c r="F23" s="18">
+        <v>96.11</v>
+      </c>
+      <c r="G23" s="18">
+        <v>122.09</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A24" s="18">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="19" t="s">
-        <v>76</v>
+      <c r="B24" s="18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C24" s="18">
+        <v>2.9750000000000001</v>
+      </c>
+      <c r="D24" s="26">
+        <v>1.3004E-59</v>
+      </c>
+      <c r="E24" s="18">
+        <v>1.1062000000000001E-2</v>
+      </c>
+      <c r="F24" s="18">
+        <v>99.55</v>
+      </c>
+      <c r="G24" s="18">
+        <v>125.54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A30" s="18" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1683,177 +1852,407 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD6F2D3E-3972-124D-B0B2-445D29279125}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="E14" sqref="A1:E14"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="29"/>
+    <col min="6" max="6" width="20.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="29" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="B1" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="B2" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="B4" s="28">
+        <v>14</v>
+      </c>
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="B5" s="30"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="B6" s="28">
+        <v>6</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="B8" s="28">
+        <v>100</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="B12" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>0.5</v>
+      </c>
+      <c r="B13" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C13" s="29">
+        <v>7.2</v>
+      </c>
+      <c r="D13" s="29">
+        <v>2.2065000000000001E-2</v>
+      </c>
+      <c r="E13" s="29">
+        <v>0.92091000000000001</v>
+      </c>
+      <c r="F13" s="29">
+        <v>11.89</v>
+      </c>
+      <c r="G13" s="29">
+        <v>24.34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>0.6</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C14" s="29">
+        <v>7.6</v>
+      </c>
+      <c r="D14" s="29">
+        <v>2.4503E-2</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0.71675999999999995</v>
+      </c>
+      <c r="F14" s="29">
+        <v>12.44</v>
+      </c>
+      <c r="G14" s="29">
+        <v>24.47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>0.7</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C15" s="29">
+        <v>7.51</v>
+      </c>
+      <c r="D15" s="29">
+        <v>2.1031000000000001E-2</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0.434</v>
+      </c>
+      <c r="F15" s="29">
+        <v>12.03</v>
+      </c>
+      <c r="G15" s="29">
+        <v>24.78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C16" s="29">
+        <v>7.42</v>
+      </c>
+      <c r="D16" s="29">
+        <v>3.5142E-2</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0.29855999999999999</v>
+      </c>
+      <c r="F16" s="29">
+        <v>12.42</v>
+      </c>
+      <c r="G16" s="29">
+        <v>26.22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="29">
+        <v>0.85</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C17" s="29">
+        <v>7.33</v>
+      </c>
+      <c r="D17" s="29">
+        <v>2.9465999999999999E-2</v>
+      </c>
+      <c r="E17" s="29">
+        <v>0.21965000000000001</v>
+      </c>
+      <c r="F17" s="29">
+        <v>12.8</v>
+      </c>
+      <c r="G17" s="29">
+        <v>30.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="29">
+        <v>0.9</v>
+      </c>
+      <c r="B18" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C18" s="29">
+        <v>7.17</v>
+      </c>
+      <c r="D18" s="29">
+        <v>2.5423999999999999E-2</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0.14649999999999999</v>
+      </c>
+      <c r="F18" s="29">
+        <v>12.39</v>
+      </c>
+      <c r="G18" s="29">
+        <v>29.87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="29">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="B19" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C19" s="29">
+        <v>7.05</v>
+      </c>
+      <c r="D19" s="29">
+        <v>2.5637E-2</v>
+      </c>
+      <c r="E19" s="29">
+        <v>9.4978999999999994E-2</v>
+      </c>
+      <c r="F19" s="29">
+        <v>12.58</v>
+      </c>
+      <c r="G19" s="29">
+        <v>31.17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="29">
+        <v>0.95</v>
+      </c>
+      <c r="B20" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C20" s="29">
+        <v>6.84</v>
+      </c>
+      <c r="D20" s="29">
+        <v>3.2819000000000001E-2</v>
+      </c>
+      <c r="E20" s="29">
+        <v>8.8696999999999998E-2</v>
+      </c>
+      <c r="F20" s="29">
+        <v>13.01</v>
+      </c>
+      <c r="G20" s="29">
+        <v>35.840000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="29">
+        <v>0.96</v>
+      </c>
+      <c r="B21" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C21" s="29">
+        <v>6.72</v>
+      </c>
+      <c r="D21" s="29">
+        <v>2.7515999999999999E-2</v>
+      </c>
+      <c r="E21" s="29">
+        <v>6.1199999999999997E-2</v>
+      </c>
+      <c r="F21" s="29">
+        <v>12.42</v>
+      </c>
+      <c r="G21" s="29">
+        <v>37.61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
+        <v>0.97</v>
+      </c>
+      <c r="B22" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C22" s="29">
+        <v>6.53</v>
+      </c>
+      <c r="D22" s="29">
+        <v>4.6115999999999997E-2</v>
+      </c>
+      <c r="E22" s="29">
+        <v>6.5724000000000005E-2</v>
+      </c>
+      <c r="F22" s="29">
+        <v>12.59</v>
+      </c>
+      <c r="G22" s="29">
+        <v>41.45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="29">
+        <v>0.98</v>
+      </c>
+      <c r="B23" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C23" s="29">
+        <v>6.25</v>
+      </c>
+      <c r="D23" s="29">
+        <v>2.7421999999999998E-2</v>
+      </c>
+      <c r="E23" s="29">
+        <v>4.6489999999999997E-2</v>
+      </c>
+      <c r="F23" s="29">
+        <v>12.67</v>
+      </c>
+      <c r="G23" s="29">
+        <v>47.64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="29">
+        <v>0.99</v>
+      </c>
+      <c r="B24" s="29">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="C24" s="29">
+        <v>5.7</v>
+      </c>
+      <c r="D24" s="29">
+        <v>2.1876E-2</v>
+      </c>
+      <c r="E24" s="29">
+        <v>2.9409999999999999E-2</v>
+      </c>
+      <c r="F24" s="29">
+        <v>12.57</v>
+      </c>
+      <c r="G24" s="29">
+        <v>62.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1861,148 +2260,250 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6D6955-E421-5547-BE42-EC892646D32C}">
-  <dimension ref="A1:E14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58CA8B3B-E8F5-E84E-AACB-62F9DECC4962}">
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" style="29" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" style="29" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" style="29" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="29" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="29"/>
+    <col min="6" max="6" width="20.6640625" style="29" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="29" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="B1" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="B2" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="B4" s="30"/>
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="B5" s="28">
+        <v>0.95</v>
+      </c>
+      <c r="C5" s="32"/>
+      <c r="D5" s="28"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="B6" s="28">
+        <v>6</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="21"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="B8" s="28">
+        <v>100</v>
+      </c>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="G12" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="29">
+        <v>10</v>
+      </c>
+      <c r="B13" s="29">
+        <v>0.92</v>
+      </c>
+      <c r="C13" s="29">
+        <v>4.5</v>
+      </c>
+      <c r="D13" s="29">
+        <v>1.0464000000000001E-3</v>
+      </c>
+      <c r="E13" s="29">
+        <v>4.8989999999999999E-2</v>
+      </c>
+      <c r="F13" s="29">
+        <v>6.07</v>
+      </c>
+      <c r="G13" s="29">
+        <v>15.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="29">
+        <v>15</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1.34</v>
+      </c>
+      <c r="C14" s="29">
+        <v>6.41</v>
+      </c>
+      <c r="D14" s="29">
+        <v>6.4724000000000004E-2</v>
+      </c>
+      <c r="E14" s="29">
+        <v>0.14524999999999999</v>
+      </c>
+      <c r="F14" s="29">
+        <v>4.34</v>
+      </c>
+      <c r="G14" s="29">
+        <v>9.8800000000000008</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="29">
+        <v>20</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1.78</v>
+      </c>
+      <c r="C15" s="29">
+        <v>8.33</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.33555000000000001</v>
+      </c>
+      <c r="E15" s="29">
+        <v>0.45044000000000001</v>
+      </c>
+      <c r="F15" s="29">
+        <v>3.05</v>
+      </c>
+      <c r="G15" s="29">
+        <v>7.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="29">
+        <v>25</v>
+      </c>
+      <c r="B16" s="29">
+        <v>2.11</v>
+      </c>
+      <c r="C16" s="29">
+        <v>9.61</v>
+      </c>
+      <c r="D16" s="29">
+        <v>0.68618999999999997</v>
+      </c>
+      <c r="E16" s="29">
+        <v>0.76575000000000004</v>
+      </c>
+      <c r="F16" s="29">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="G16" s="29">
+        <v>5.57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="29">
+        <v>28</v>
+      </c>
+      <c r="B17" s="29">
+        <v>9.91</v>
+      </c>
+      <c r="C17" s="29">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D17" s="29">
+        <v>2.0217000000000001</v>
+      </c>
+      <c r="E17" s="29">
+        <v>2.1930999999999998</v>
+      </c>
+      <c r="F17" s="29">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="G17" s="29">
+        <v>6.19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>